<commit_message>
Final Phase 1 Submission: Added Progress Report and updated work logs
</commit_message>
<xml_diff>
--- a/DocumentAndReports/Work Log.xlsx
+++ b/DocumentAndReports/Work Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://collegedouglas-my.sharepoint.com/personal/silvas1_student_douglascollege_ca/Documents/Applied Research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandali Silva\Documents\GitHub\W26_4495_S2_SandaliS\DocumentAndReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E56E2620-870E-4430-8DD1-08E200E3177B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D76B7A-F5D4-4E01-80DC-9BC3BE6AE0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Work Log" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Prompts" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="145">
   <si>
     <t>Date</t>
   </si>
@@ -270,6 +269,253 @@
   </si>
   <si>
     <t>Logo creation</t>
+  </si>
+  <si>
+    <t>Progress report structuring</t>
+  </si>
+  <si>
+    <t>“Provide a format for Progress Report 1 for a system development project”</t>
+  </si>
+  <si>
+    <t>Selected only sections required by course guidelines and adapted structure to reflect SafeSight’s early development stage</t>
+  </si>
+  <si>
+    <t>Milestone planning</t>
+  </si>
+  <si>
+    <t>“Identify suitable milestones for Phase 1 of a predictive system project”</t>
+  </si>
+  <si>
+    <t>Refined milestones to align with completed research activities and realistic academic timelines</t>
+  </si>
+  <si>
+    <t>Scope clarification</t>
+  </si>
+  <si>
+    <t>“Explain how to define project scope for an applied IT research project”</t>
+  </si>
+  <si>
+    <t>Clarified system boundaries and excluded advanced features not feasible within course duration</t>
+  </si>
+  <si>
+    <t>Requirement prioritisation</t>
+  </si>
+  <si>
+    <t>“How to prioritise functional requirements for an MVP system”</t>
+  </si>
+  <si>
+    <t>Evaluated suggested requirements and selected core safety analytics features for initial implementation</t>
+  </si>
+  <si>
+    <t>Risk and issue identification</t>
+  </si>
+  <si>
+    <t>“Common early-stage risks in system development projects”</t>
+  </si>
+  <si>
+    <t>Identified relevant risks and documented mitigation strategies applicable to SafeSight development</t>
+  </si>
+  <si>
+    <t>Academic reflection support</t>
+  </si>
+  <si>
+    <t>“How to write reflective progress for an IT project”</t>
+  </si>
+  <si>
+    <t>Rewrote content in own words, ensuring critical reflection rather than descriptive reporting</t>
+  </si>
+  <si>
+    <t>Alignment check</t>
+  </si>
+  <si>
+    <t>“How to align progress reports with original project proposal”</t>
+  </si>
+  <si>
+    <t>Cross-checked progress against proposal objectives and adjusted report to maintain consistency</t>
+  </si>
+  <si>
+    <t>Database design guidance</t>
+  </si>
+  <si>
+    <t>“Suggest database structure for a workplace safety analytics system”</t>
+  </si>
+  <si>
+    <t>Reviewed proposed schema, normalised tables, and selected entities relevant to hospitality safety incidents</t>
+  </si>
+  <si>
+    <t>Data modelling explanation</t>
+  </si>
+  <si>
+    <t>“Explain relational vs analytical database models”</t>
+  </si>
+  <si>
+    <t>Chose relational model for transactional safety data and justified design choice in report</t>
+  </si>
+  <si>
+    <t>Dataset cleaning guidance</t>
+  </si>
+  <si>
+    <t>“How to clean and prepare incident datasets for predictive analysis”</t>
+  </si>
+  <si>
+    <t>Applied only applicable cleaning steps and excluded unrealistic transformations for simulated data</t>
+  </si>
+  <si>
+    <t>Data validation rules</t>
+  </si>
+  <si>
+    <t>“What validation checks are required for safety datasets”</t>
+  </si>
+  <si>
+    <t>Defined validation rules aligned with workplace incident reporting standards</t>
+  </si>
+  <si>
+    <t>Front-end architecture explanation</t>
+  </si>
+  <si>
+    <t>“Explain front-end architecture for a data dashboard”</t>
+  </si>
+  <si>
+    <t>Selected dashboard-based UI approach suitable for managers and HR users</t>
+  </si>
+  <si>
+    <t>Back-end design support</t>
+  </si>
+  <si>
+    <t>“Describe back-end services for analytics systems”</t>
+  </si>
+  <si>
+    <t>Mapped suggested services to a simplified API structure appropriate for course scope</t>
+  </si>
+  <si>
+    <t>API design guidance</t>
+  </si>
+  <si>
+    <t>“Design REST API endpoints for a safety reporting system”</t>
+  </si>
+  <si>
+    <t>Filtered endpoints to core MVP features and documented them at a conceptual level</t>
+  </si>
+  <si>
+    <t>Environment setup guidance</t>
+  </si>
+  <si>
+    <t>“Development environment setup for full-stack analytics project”</t>
+  </si>
+  <si>
+    <t>Selected tools and configurations compatible with local machine and institutional constraints</t>
+  </si>
+  <si>
+    <t>Deployment awareness</t>
+  </si>
+  <si>
+    <t>“Common deployment considerations for academic system projects”</t>
+  </si>
+  <si>
+    <t>Identified constraints and documented limitations rather than attempting premature deployment</t>
+  </si>
+  <si>
+    <t>Dataset cleaning and SQL import</t>
+  </si>
+  <si>
+    <t>Mandatory consultation with supervisor</t>
+  </si>
+  <si>
+    <t>Discussed project direction and received guidance to obtain operational requirements from Fairmont Waterfront</t>
+  </si>
+  <si>
+    <t>Development environment setup</t>
+  </si>
+  <si>
+    <t>Configured local development environment and required tools for system development</t>
+  </si>
+  <si>
+    <t>Meeting with Fairmont Waterfront HR department</t>
+  </si>
+  <si>
+    <t>Collected operational insights from HR to prioritise system features, as advised by the supervisor</t>
+  </si>
+  <si>
+    <t>Dataset and industry research</t>
+  </si>
+  <si>
+    <t>Conducted in-depth research on relevant datasets and reviewed comparable workplace safety systems</t>
+  </si>
+  <si>
+    <t>Dashboard feature research</t>
+  </si>
+  <si>
+    <t>Analysed and shortlisted core features required for the SafeSight dashboard</t>
+  </si>
+  <si>
+    <t>Cleaned selected datasets and prepared them for import into the SQL database</t>
+  </si>
+  <si>
+    <t>SafeSight data preparation (Jupyter Notebook)</t>
+  </si>
+  <si>
+    <t>Developed and documented data preparation steps using a Jupyter Notebook</t>
+  </si>
+  <si>
+    <t>Progress Report 1 finalisation</t>
+  </si>
+  <si>
+    <t>Compiled, reviewed, and finalised Progress Report 1 for submission</t>
+  </si>
+  <si>
+    <t>Developed Backend (Application Layer) using Node.js and Express.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Installed dependencies and wrote </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>index.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for DB connectivity.</t>
+    </r>
+  </si>
+  <si>
+    <t>Integrated React.js Frontend (Presentation Layer).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Scaffolded the React app inside the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>FrontEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> directory.</t>
+    </r>
+  </si>
+  <si>
+    <t>Verified Full-Stack connection and committed changes to GitHub. Confirmed "Connected to SafeSight MySQL Database" in terminal.</t>
   </si>
 </sst>
 </file>
@@ -279,7 +525,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +540,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -344,7 +595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -368,17 +619,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -402,31 +689,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -441,45 +704,41 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41F59F99-6A6B-4C90-994D-BBFEB2BDE46C}" name="Table1" displayName="Table1" ref="A1:D128" totalsRowShown="0">
-  <autoFilter ref="A1:D128" xr:uid="{41F59F99-6A6B-4C90-994D-BBFEB2BDE46C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41F59F99-6A6B-4C90-994D-BBFEB2BDE46C}" name="Table1" displayName="Table1" ref="A1:D130" totalsRowShown="0">
+  <autoFilter ref="A1:D130" xr:uid="{41F59F99-6A6B-4C90-994D-BBFEB2BDE46C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5ABDF1AC-6CA2-4D3D-BED1-ABBE8632EF5A}" name="Date" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{48C587D8-0357-4367-9662-FE4DF7A0731E}" name="Number of Hours" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{423E5E18-754F-4F31-A0AF-8A6961646D3E}" name="Description"/>
-    <tableColumn id="4" xr3:uid="{4D463411-D60A-45E9-A354-72F630B4F08F}" name="Remarks"/>
+    <tableColumn id="1" xr3:uid="{5ABDF1AC-6CA2-4D3D-BED1-ABBE8632EF5A}" name="Date" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{48C587D8-0357-4367-9662-FE4DF7A0731E}" name="Number of Hours" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{423E5E18-754F-4F31-A0AF-8A6961646D3E}" name="Description" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{4D463411-D60A-45E9-A354-72F630B4F08F}" name="Remarks" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{62A78FFA-69C1-4830-8948-7A15783C8983}" name="Table3" displayName="Table3" ref="A1:E1048576" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:E1048576" xr:uid="{62A78FFA-69C1-4830-8948-7A15783C8983}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{62A78FFA-69C1-4830-8948-7A15783C8983}" name="Table3" displayName="Table3" ref="A1:E1048574" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:E1048574" xr:uid="{62A78FFA-69C1-4830-8948-7A15783C8983}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7720FBCA-9D18-4AA6-AD20-22B601758C3E}" name="AI Tool Name" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{8D78E618-FCAF-4D63-B328-64EF4380AEB4}" name="Version / Account Type" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B99F606B-3981-4DF0-80B0-82F9716EEB6E}" name="Specific Feature Used" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{C60CFB0A-096D-48E4-BBCB-28DF6594EBFA}" name="Prompt Used (Summary)" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{5423605D-7B52-4200-9789-A3D7EF34731D}" name="Value Addition (Student Contribution)" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{7720FBCA-9D18-4AA6-AD20-22B601758C3E}" name="AI Tool Name" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{8D78E618-FCAF-4D63-B328-64EF4380AEB4}" name="Version / Account Type" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{B99F606B-3981-4DF0-80B0-82F9716EEB6E}" name="Specific Feature Used" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{C60CFB0A-096D-48E4-BBCB-28DF6594EBFA}" name="Prompt Used (Summary)" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{5423605D-7B52-4200-9789-A3D7EF34731D}" name="Value Addition (Student Contribution)" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{222BE556-30D3-471B-AED8-DC62DCF03F3B}" name="Table2" displayName="Table2" ref="A1:E38" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{222BE556-30D3-471B-AED8-DC62DCF03F3B}" name="Table2" displayName="Table2" ref="A1:E38" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:E38" xr:uid="{222BE556-30D3-471B-AED8-DC62DCF03F3B}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BE6E2BDB-D181-4A5D-951F-7374EF1C522E}" name="AI Tool name"/>
     <tableColumn id="2" xr3:uid="{C4FB3244-0677-4814-A164-D1E7377C7283}" name="Version, Account type"/>
     <tableColumn id="3" xr3:uid="{7DA1642C-E6C1-4F23-AE7D-99FAE70CFD8F}" name="Specific feature for which the AI tool was used"/>
-    <tableColumn id="5" xr3:uid="{66FA771B-4EAF-4509-BBFE-B3169E286681}" name="Prompt" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{66FA771B-4EAF-4509-BBFE-B3169E286681}" name="Prompt" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{F95B88AB-6922-4465-B5A8-FB049FCB1F6F}" name="Value Addition_x000a_What value did you add over and above what AI did for you?"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -783,20 +1042,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="24.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.5546875" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="36.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -810,21 +1069,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="57.6">
       <c r="A2" s="1">
         <v>46031</v>
       </c>
       <c r="B2" s="6">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="43.2">
       <c r="A3" s="1">
         <v>46032</v>
       </c>
@@ -834,8 +1093,9 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="28.8">
       <c r="A4" s="1">
         <v>46034</v>
       </c>
@@ -845,8 +1105,9 @@
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="57.6">
       <c r="A5" s="1">
         <v>46037</v>
       </c>
@@ -856,8 +1117,9 @@
       <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="28.8">
       <c r="A6" s="1">
         <v>46038</v>
       </c>
@@ -867,61 +1129,651 @@
       <c r="C6" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>46042</v>
       </c>
       <c r="B7" s="6">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>46043</v>
       </c>
       <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>46044</v>
       </c>
       <c r="B9" s="6">
         <v>0.5</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>46046</v>
       </c>
       <c r="B10" s="6">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>46047</v>
       </c>
       <c r="B11" s="6">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="43.2">
+      <c r="A12" s="12">
+        <v>46052</v>
+      </c>
+      <c r="B12" s="11">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="43.2">
+      <c r="A13" s="12">
+        <v>46054</v>
+      </c>
+      <c r="B13" s="11">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="43.2">
+      <c r="A14" s="12">
+        <v>46055</v>
+      </c>
+      <c r="B14" s="11">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8">
+      <c r="A15" s="12">
+        <v>46056</v>
+      </c>
+      <c r="B15" s="6">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="43.2">
+      <c r="A16" s="12">
+        <v>46057</v>
+      </c>
+      <c r="B16" s="11">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8">
+      <c r="A17" s="12">
+        <v>46058</v>
+      </c>
+      <c r="B17" s="11">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.8">
+      <c r="A18" s="12">
+        <v>46059</v>
+      </c>
+      <c r="B18" s="11">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="28.8">
+      <c r="A19" s="12">
+        <v>46060</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="57.6">
+      <c r="A20" s="12">
+        <v>46060</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" ht="43.2">
+      <c r="A21" s="12">
+        <v>46061</v>
+      </c>
+      <c r="B21" s="11">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.8">
+      <c r="A22" s="12">
+        <v>46062</v>
+      </c>
+      <c r="B22" s="11">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="3:4">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="3:4">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="3:4">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="3:4">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="3:4">
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="3:4">
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="3:4">
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="3:4">
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="3:4">
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="3:4">
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="3:4">
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="3:4">
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="3:4">
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="3:4">
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="3:4">
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="3:4">
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="3:4">
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="3:4">
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="3:4">
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="3:4">
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="3:4">
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="3:4">
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="3:4">
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="3:4">
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="3:4">
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="3:4">
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="3:4">
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="3:4">
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="3:4">
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="3:4">
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="3:4">
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+    </row>
+    <row r="64" spans="3:4">
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="3:4">
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="3:4">
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="3:4">
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="3:4">
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="3:4">
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="3:4">
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="3:4">
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="3:4">
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="3:4">
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="3:4">
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="3:4">
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="3:4">
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="3:4">
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="3:4">
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="3:4">
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="3:4">
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="3:4">
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="3:4">
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="3:4">
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="3:4">
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="3:4">
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="3:4">
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="3:4">
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="3:4">
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="3:4">
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="3:4">
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+    </row>
+    <row r="91" spans="3:4">
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+    </row>
+    <row r="92" spans="3:4">
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+    </row>
+    <row r="93" spans="3:4">
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+    </row>
+    <row r="94" spans="3:4">
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="3:4">
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="3:4">
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="3:4">
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+    </row>
+    <row r="98" spans="3:4">
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="3:4">
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+    </row>
+    <row r="100" spans="3:4">
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="3:4">
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+    </row>
+    <row r="102" spans="3:4">
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+    </row>
+    <row r="103" spans="3:4">
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+    </row>
+    <row r="104" spans="3:4">
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+    </row>
+    <row r="105" spans="3:4">
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="3:4">
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+    </row>
+    <row r="107" spans="3:4">
+      <c r="C107" s="2"/>
+      <c r="D107" s="2"/>
+    </row>
+    <row r="108" spans="3:4">
+      <c r="C108" s="2"/>
+      <c r="D108" s="2"/>
+    </row>
+    <row r="109" spans="3:4">
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+    </row>
+    <row r="110" spans="3:4">
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+    </row>
+    <row r="111" spans="3:4">
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+    </row>
+    <row r="112" spans="3:4">
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+    </row>
+    <row r="113" spans="3:4">
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+    </row>
+    <row r="114" spans="3:4">
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
+    </row>
+    <row r="115" spans="3:4">
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
+    </row>
+    <row r="116" spans="3:4">
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+    </row>
+    <row r="117" spans="3:4">
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+    </row>
+    <row r="118" spans="3:4">
+      <c r="C118" s="2"/>
+      <c r="D118" s="2"/>
+    </row>
+    <row r="119" spans="3:4">
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+    </row>
+    <row r="120" spans="3:4">
+      <c r="C120" s="2"/>
+      <c r="D120" s="2"/>
+    </row>
+    <row r="121" spans="3:4">
+      <c r="C121" s="2"/>
+      <c r="D121" s="2"/>
+    </row>
+    <row r="122" spans="3:4">
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
+    </row>
+    <row r="123" spans="3:4">
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
+    </row>
+    <row r="124" spans="3:4">
+      <c r="C124" s="2"/>
+      <c r="D124" s="2"/>
+    </row>
+    <row r="125" spans="3:4">
+      <c r="C125" s="2"/>
+      <c r="D125" s="2"/>
+    </row>
+    <row r="126" spans="3:4">
+      <c r="C126" s="2"/>
+      <c r="D126" s="2"/>
+    </row>
+    <row r="127" spans="3:4">
+      <c r="C127" s="2"/>
+      <c r="D127" s="2"/>
+    </row>
+    <row r="128" spans="3:4">
+      <c r="C128" s="2"/>
+      <c r="D128" s="2"/>
+    </row>
+    <row r="129" spans="3:4">
+      <c r="C129" s="2"/>
+      <c r="D129" s="2"/>
+    </row>
+    <row r="130" spans="3:4">
+      <c r="C130" s="2"/>
+      <c r="D130" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -933,22 +1785,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40EA87B-8D49-4A90-9FD7-CCB75014BEFC}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.21875" style="8" customWidth="1"/>
     <col min="2" max="2" width="22.5546875" style="8" customWidth="1"/>
     <col min="3" max="3" width="20.77734375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="34.88671875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="23.77734375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="7" t="s">
         <v>27</v>
       </c>
@@ -965,7 +1817,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="57.6">
       <c r="A2" s="4" t="s">
         <v>32</v>
       </c>
@@ -982,7 +1834,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="43.2">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -999,7 +1851,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="43.2">
       <c r="A4" s="4" t="s">
         <v>32</v>
       </c>
@@ -1016,7 +1868,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="43.2">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -1033,7 +1885,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="43.2">
       <c r="A6" s="4" t="s">
         <v>32</v>
       </c>
@@ -1050,7 +1902,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="43.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
@@ -1067,7 +1919,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="43.2">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -1084,7 +1936,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="43.2">
       <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
@@ -1101,7 +1953,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="43.2">
       <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
@@ -1118,7 +1970,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="28.8">
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
@@ -1135,7 +1987,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="43.2">
       <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
@@ -1152,7 +2004,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="29.4" thickBot="1">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
@@ -1169,7 +2021,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="43.8" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>73</v>
       </c>
@@ -1181,6 +2033,278 @@
       </c>
       <c r="D14" s="4" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="43.2">
+      <c r="A15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="43.2">
+      <c r="A16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="43.2">
+      <c r="A17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="43.2">
+      <c r="A18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="43.2">
+      <c r="A19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="43.2">
+      <c r="A20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="43.2">
+      <c r="A21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="43.2">
+      <c r="A22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="43.2">
+      <c r="A23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="57.6">
+      <c r="A24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="43.2">
+      <c r="A25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="43.2">
+      <c r="A26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="43.2">
+      <c r="A27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="43.2">
+      <c r="A28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="43.2">
+      <c r="A29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="43.2">
+      <c r="A30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1199,7 +2323,7 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1213,7 +2337,7 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="10.44140625" customWidth="1"/>
     <col min="2" max="2" width="21.44140625" customWidth="1"/>
@@ -1222,7 +2346,7 @@
     <col min="5" max="5" width="50.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="94.8" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1239,64 +2363,64 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="C2" s="2"/>
       <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="D3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="D6" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="28.8">
       <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="28.8">
       <c r="D8" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="D9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="D10" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="D11" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="D12" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="D13" s="4" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Objective 1: Established role-based routing and modular component structure for SafeSight
</commit_message>
<xml_diff>
--- a/DocumentAndReports/Work Log.xlsx
+++ b/DocumentAndReports/Work Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandali Silva\Documents\GitHub\W26_4495_S2_SandaliS\DocumentAndReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D76B7A-F5D4-4E01-80DC-9BC3BE6AE0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29650A1-7408-462A-B302-A8F770F3F7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="149">
   <si>
     <t>Date</t>
   </si>
@@ -516,6 +516,18 @@
   </si>
   <si>
     <t>Verified Full-Stack connection and committed changes to GitHub. Confirmed "Connected to SafeSight MySQL Database" in terminal.</t>
+  </si>
+  <si>
+    <t>Phase 2 headstart with bridging presentation layer and the data layer</t>
+  </si>
+  <si>
+    <t>Gemini</t>
+  </si>
+  <si>
+    <t>"Troubleshooting Node"</t>
+  </si>
+  <si>
+    <t>"Bridging the layers"</t>
   </si>
 </sst>
 </file>
@@ -637,15 +649,6 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -689,6 +692,15 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     </dxf>
   </dxfs>
@@ -709,36 +721,36 @@
   <autoFilter ref="A1:D130" xr:uid="{41F59F99-6A6B-4C90-994D-BBFEB2BDE46C}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5ABDF1AC-6CA2-4D3D-BED1-ABBE8632EF5A}" name="Date" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{48C587D8-0357-4367-9662-FE4DF7A0731E}" name="Number of Hours" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{423E5E18-754F-4F31-A0AF-8A6961646D3E}" name="Description" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{4D463411-D60A-45E9-A354-72F630B4F08F}" name="Remarks" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{48C587D8-0357-4367-9662-FE4DF7A0731E}" name="Number of Hours" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{423E5E18-754F-4F31-A0AF-8A6961646D3E}" name="Description" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{4D463411-D60A-45E9-A354-72F630B4F08F}" name="Remarks" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{62A78FFA-69C1-4830-8948-7A15783C8983}" name="Table3" displayName="Table3" ref="A1:E1048574" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{62A78FFA-69C1-4830-8948-7A15783C8983}" name="Table3" displayName="Table3" ref="A1:E1048574" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:E1048574" xr:uid="{62A78FFA-69C1-4830-8948-7A15783C8983}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{7720FBCA-9D18-4AA6-AD20-22B601758C3E}" name="AI Tool Name" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{8D78E618-FCAF-4D63-B328-64EF4380AEB4}" name="Version / Account Type" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{B99F606B-3981-4DF0-80B0-82F9716EEB6E}" name="Specific Feature Used" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{C60CFB0A-096D-48E4-BBCB-28DF6594EBFA}" name="Prompt Used (Summary)" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{5423605D-7B52-4200-9789-A3D7EF34731D}" name="Value Addition (Student Contribution)" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{7720FBCA-9D18-4AA6-AD20-22B601758C3E}" name="AI Tool Name" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{8D78E618-FCAF-4D63-B328-64EF4380AEB4}" name="Version / Account Type" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{B99F606B-3981-4DF0-80B0-82F9716EEB6E}" name="Specific Feature Used" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{C60CFB0A-096D-48E4-BBCB-28DF6594EBFA}" name="Prompt Used (Summary)" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{5423605D-7B52-4200-9789-A3D7EF34731D}" name="Value Addition (Student Contribution)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{222BE556-30D3-471B-AED8-DC62DCF03F3B}" name="Table2" displayName="Table2" ref="A1:E38" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{222BE556-30D3-471B-AED8-DC62DCF03F3B}" name="Table2" displayName="Table2" ref="A1:E38" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:E38" xr:uid="{222BE556-30D3-471B-AED8-DC62DCF03F3B}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{BE6E2BDB-D181-4A5D-951F-7374EF1C522E}" name="AI Tool name"/>
     <tableColumn id="2" xr3:uid="{C4FB3244-0677-4814-A164-D1E7377C7283}" name="Version, Account type"/>
     <tableColumn id="3" xr3:uid="{7DA1642C-E6C1-4F23-AE7D-99FAE70CFD8F}" name="Specific feature for which the AI tool was used"/>
-    <tableColumn id="5" xr3:uid="{66FA771B-4EAF-4509-BBFE-B3169E286681}" name="Prompt" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{66FA771B-4EAF-4509-BBFE-B3169E286681}" name="Prompt" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{F95B88AB-6922-4465-B5A8-FB049FCB1F6F}" name="Value Addition_x000a_What value did you add over and above what AI did for you?"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1044,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1343,8 +1355,16 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="C23" s="2"/>
+    <row r="23" spans="1:4" ht="28.8">
+      <c r="A23" s="12">
+        <v>46062</v>
+      </c>
+      <c r="B23" s="6">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:4">
@@ -1785,10 +1805,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40EA87B-8D49-4A90-9FD7-CCB75014BEFC}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2305,6 +2325,22 @@
       </c>
       <c r="E30" s="3" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>